<commit_message>
Electron velocity and plasma potential calculations
</commit_message>
<xml_diff>
--- a/Plasma/argonData_Paschen.xlsx
+++ b/Plasma/argonData_Paschen.xlsx
@@ -1,33 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yao\Documents\GitHub\Physics_191\Plasma\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C59CDA-59D2-400A-B37F-BED8113D5217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -52,143 +34,143 @@
     <t>V_B</t>
   </si>
   <si>
-    <t>Data/Paschen\Argon_121mTrange50-1000V.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_131mTrange50-1000V.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_137mTrange50-1000V.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_282mTrange50-1000V.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_282mTrange50-1000V_2.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_364mTrange50-1000V_1.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_364mTrange50-1000V_2.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_364mTrange50-1000V_3.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_364mTrange50-1000V_4.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_364mTrange50-1000V_5.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_364mTrange50-1000V_6.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_536mTrange200-600V_1.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_536mTrange50-1000V_1.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_71mTrange200-600V_1.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_71mTrange200-600V_2.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_71mTrange200-600V_3.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_71mTrange200-600V_4.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_71mTrange200-600V_5.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_71mTrange200-600V_6.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_100mT.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_192mT.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_192mT_1.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_192mT_2.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_192mT_3.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_192mT_4.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_192mT_5.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_371mT.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_371mT_1.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_371mT_2.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_371mT_3.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_371mT_4.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_371mT_5.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_449mT_1.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_449mT_2.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_449mT_3.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_449mT_4.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_449mT_5.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_449mT_6.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_700mT_1.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_700mT_2.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_700mT_3.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_700mT_4.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_700mT_5.txt</t>
-  </si>
-  <si>
-    <t>Data/Paschen\Argon_PaschenCurve_700mT_6.txt</t>
+    <t>Data/Paschen/Argon_282mTrange50-1000V.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_700mT_4.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_449mT_5.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_449mT_4.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_700mT_5.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_371mT.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_192mT.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_449mT_6.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_700mT_6.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_700mT_2.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_449mT_3.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_449mT_2.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_700mT_3.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_700mT_1.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_282mTrange50-1000V_2.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_449mT_1.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_371mT_1.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_536mTrange50-1000V_1.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_71mTrange200-600V_2.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_192mT_3.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_364mTrange50-1000V_1.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_192mT_2.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_71mTrange200-600V_3.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_371mT_2.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_131mTrange50-1000V.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_71mTrange200-600V_1.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_364mTrange50-1000V_2.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_364mTrange50-1000V_3.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_121mTrange50-1000V.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_192mT_1.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_371mT_3.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_71mTrange200-600V_4.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_192mT_5.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_364mTrange50-1000V_6.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_192mT_4.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_71mTrange200-600V_5.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_371mT_4.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_364mTrange50-1000V_4.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_364mTrange50-1000V_5.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_536mTrange200-600V_1.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_71mTrange200-600V_6.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_100mT.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_PaschenCurve_371mT_5.txt</t>
+  </si>
+  <si>
+    <t>Data/Paschen/Argon_137mTrange50-1000V.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,14 +233,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -305,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -337,27 +311,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,24 +345,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -582,22 +520,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -625,7 +555,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>121</v>
+        <v>282</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -637,21 +567,10 @@
         <v>0.3</v>
       </c>
       <c r="G2">
-        <v>-428.68299300000001</v>
-      </c>
-      <c r="H2">
-        <f t="shared" ref="H2:H7" si="0">C2</f>
-        <v>121</v>
-      </c>
-      <c r="I2">
-        <f>G2</f>
-        <v>-428.68299300000001</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-347.946876</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -659,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>131</v>
+        <v>700</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -671,21 +590,10 @@
         <v>0.3</v>
       </c>
       <c r="G3">
-        <v>-456.902625</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
-        <v>131</v>
-      </c>
-      <c r="I3">
-        <f>G3</f>
-        <v>-456.902625</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-266.336142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -693,7 +601,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>137</v>
+        <v>449</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -705,21 +613,10 @@
         <v>0.3</v>
       </c>
       <c r="G4">
-        <v>-456.997681</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>137</v>
-      </c>
-      <c r="I4">
-        <f>G4</f>
-        <v>-456.997681</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-254.573919</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -727,7 +624,7 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>282</v>
+        <v>449</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -739,21 +636,10 @@
         <v>0.3</v>
       </c>
       <c r="G5">
-        <v>-347.94687599999997</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>282</v>
-      </c>
-      <c r="I5">
-        <f t="shared" ref="I5:I6" si="1">G5</f>
-        <v>-347.94687599999997</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-252.855909</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -761,7 +647,7 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>282</v>
+        <v>700</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -773,21 +659,10 @@
         <v>0.3</v>
       </c>
       <c r="G6">
-        <v>-345.99070399999999</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>282</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>-345.99070399999999</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-266.659579</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -795,7 +670,7 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -807,22 +682,10 @@
         <v>0.3</v>
       </c>
       <c r="G7">
-        <v>-288.53617500000001</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>364</v>
-      </c>
-      <c r="I7">
-        <f>AVERAGE(G7:G12)</f>
-        <v>-285.55993033333334</v>
-      </c>
-      <c r="J7">
-        <f>_xlfn.STDEV.P(G7:G12)</f>
-        <v>4.1514389886956335</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-269.75942</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -830,7 +693,7 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>364</v>
+        <v>192</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -842,10 +705,10 @@
         <v>0.3</v>
       </c>
       <c r="G8">
-        <v>-292.71020199999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-245.704896</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -853,7 +716,7 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>364</v>
+        <v>449</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -865,10 +728,10 @@
         <v>0.3</v>
       </c>
       <c r="G9">
-        <v>-285.55526600000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-255.581733</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -876,7 +739,7 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>364</v>
+        <v>700</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -888,10 +751,10 @@
         <v>0.3</v>
       </c>
       <c r="G10">
-        <v>-284.627274</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-266.948454</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -899,7 +762,7 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>364</v>
+        <v>700</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -911,10 +774,10 @@
         <v>0.3</v>
       </c>
       <c r="G11">
-        <v>-281.37259699999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-262.633294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -922,7 +785,7 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>364</v>
+        <v>449</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -934,10 +797,10 @@
         <v>0.3</v>
       </c>
       <c r="G12">
-        <v>-280.55806799999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-253.55488</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -945,7 +808,7 @@
         <v>17</v>
       </c>
       <c r="C13">
-        <v>536</v>
+        <v>449</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -957,21 +820,10 @@
         <v>0.3</v>
       </c>
       <c r="G13">
-        <v>-276.56829699999997</v>
-      </c>
-      <c r="H13">
-        <f>C13</f>
-        <v>536</v>
-      </c>
-      <c r="I13">
-        <f t="shared" ref="I13:I14" si="2">G13</f>
-        <v>-276.56829699999997</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-251.899849</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -979,7 +831,7 @@
         <v>18</v>
       </c>
       <c r="C14">
-        <v>536</v>
+        <v>700</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -991,21 +843,10 @@
         <v>0.3</v>
       </c>
       <c r="G14">
-        <v>-318.78217699999999</v>
-      </c>
-      <c r="H14">
-        <f>C14</f>
-        <v>536</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="2"/>
-        <v>-318.78217699999999</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-257.794327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1013,7 +854,7 @@
         <v>19</v>
       </c>
       <c r="C15">
-        <v>71</v>
+        <v>700</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -1025,22 +866,10 @@
         <v>0.3</v>
       </c>
       <c r="G15">
-        <v>-462.77988499999998</v>
-      </c>
-      <c r="H15">
-        <f>C15</f>
-        <v>71</v>
-      </c>
-      <c r="I15">
-        <f>AVERAGE(G15:G20)</f>
-        <v>-468.89589933333332</v>
-      </c>
-      <c r="J15">
-        <f>_xlfn.STDEV.P(G15:G20)</f>
-        <v>4.3316902298515396</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-261.799654</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1048,7 +877,7 @@
         <v>20</v>
       </c>
       <c r="C16">
-        <v>71</v>
+        <v>282</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -1060,10 +889,10 @@
         <v>0.3</v>
       </c>
       <c r="G16">
-        <v>-465.40706</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-345.990704</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1071,7 +900,7 @@
         <v>21</v>
       </c>
       <c r="C17">
-        <v>71</v>
+        <v>449</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -1083,10 +912,10 @@
         <v>0.3</v>
       </c>
       <c r="G17">
-        <v>-465.95484099999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-252.364601</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1094,7 +923,7 @@
         <v>22</v>
       </c>
       <c r="C18">
-        <v>71</v>
+        <v>371</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -1106,10 +935,10 @@
         <v>0.3</v>
       </c>
       <c r="G18">
-        <v>-472.09296799999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-268.196066</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1117,7 +946,7 @@
         <v>23</v>
       </c>
       <c r="C19">
-        <v>71</v>
+        <v>536</v>
       </c>
       <c r="D19">
         <v>5</v>
@@ -1129,10 +958,10 @@
         <v>0.3</v>
       </c>
       <c r="G19">
-        <v>-473.10550799999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-318.782177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1152,10 +981,10 @@
         <v>0.3</v>
       </c>
       <c r="G20">
-        <v>-474.03513400000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-465.40706</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1163,7 +992,7 @@
         <v>25</v>
       </c>
       <c r="C21">
-        <v>100</v>
+        <v>192</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -1175,21 +1004,10 @@
         <v>0.3</v>
       </c>
       <c r="G21">
-        <v>-580.64300800000001</v>
-      </c>
-      <c r="H21">
-        <f>C21</f>
-        <v>100</v>
-      </c>
-      <c r="I21">
-        <f>G21</f>
-        <v>-580.64300800000001</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-246.809326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1197,7 +1015,7 @@
         <v>26</v>
       </c>
       <c r="C22">
-        <v>192</v>
+        <v>364</v>
       </c>
       <c r="D22">
         <v>5</v>
@@ -1209,22 +1027,10 @@
         <v>0.3</v>
       </c>
       <c r="G22">
-        <v>-245.70489599999999</v>
-      </c>
-      <c r="H22">
-        <f>C22</f>
-        <v>192</v>
-      </c>
-      <c r="I22">
-        <f>AVERAGE(G22:G27)</f>
-        <v>-246.29728899999998</v>
-      </c>
-      <c r="J22">
-        <f>_xlfn.STDEV.P(G22:G27)</f>
-        <v>0.68781788248513676</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-288.536175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1244,10 +1050,10 @@
         <v>0.3</v>
       </c>
       <c r="G23">
-        <v>-246.19262000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-246.5328</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1255,7 +1061,7 @@
         <v>28</v>
       </c>
       <c r="C24">
-        <v>192</v>
+        <v>71</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -1267,10 +1073,10 @@
         <v>0.3</v>
       </c>
       <c r="G24">
-        <v>-246.53280000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-465.954841</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1278,7 +1084,7 @@
         <v>29</v>
       </c>
       <c r="C25">
-        <v>192</v>
+        <v>371</v>
       </c>
       <c r="D25">
         <v>5</v>
@@ -1290,10 +1096,10 @@
         <v>0.3</v>
       </c>
       <c r="G25">
-        <v>-246.809326</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-266.81769</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1301,7 +1107,7 @@
         <v>30</v>
       </c>
       <c r="C26">
-        <v>192</v>
+        <v>131</v>
       </c>
       <c r="D26">
         <v>5</v>
@@ -1313,10 +1119,10 @@
         <v>0.3</v>
       </c>
       <c r="G26">
-        <v>-245.23335599999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-456.902625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1324,7 +1130,7 @@
         <v>31</v>
       </c>
       <c r="C27">
-        <v>192</v>
+        <v>71</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -1336,10 +1142,10 @@
         <v>0.3</v>
       </c>
       <c r="G27">
-        <v>-247.31073599999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-462.779885</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1347,7 +1153,7 @@
         <v>32</v>
       </c>
       <c r="C28">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="D28">
         <v>5</v>
@@ -1359,22 +1165,10 @@
         <v>0.3</v>
       </c>
       <c r="G28">
-        <v>-269.75941999999998</v>
-      </c>
-      <c r="H28">
-        <f>C28</f>
-        <v>371</v>
-      </c>
-      <c r="I28">
-        <f>AVERAGE(G28:G33)</f>
-        <v>-266.7758363333333</v>
-      </c>
-      <c r="J28">
-        <f>_xlfn.STDEV.P(G28:G33)</f>
-        <v>1.7476932300124013</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-292.710202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1382,7 +1176,7 @@
         <v>33</v>
       </c>
       <c r="C29">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="D29">
         <v>5</v>
@@ -1394,10 +1188,10 @@
         <v>0.3</v>
       </c>
       <c r="G29">
-        <v>-268.19606599999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-285.555266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1405,7 +1199,7 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <v>371</v>
+        <v>121</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -1417,10 +1211,10 @@
         <v>0.3</v>
       </c>
       <c r="G30">
-        <v>-266.81769000000003</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-428.682993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1428,7 +1222,7 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>371</v>
+        <v>192</v>
       </c>
       <c r="D31">
         <v>5</v>
@@ -1440,10 +1234,10 @@
         <v>0.3</v>
       </c>
       <c r="G31">
-        <v>-265.91985199999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-246.19262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1463,10 +1257,10 @@
         <v>0.3</v>
       </c>
       <c r="G32">
-        <v>-265.320402</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-265.919852</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1474,7 +1268,7 @@
         <v>37</v>
       </c>
       <c r="C33">
-        <v>371</v>
+        <v>71</v>
       </c>
       <c r="D33">
         <v>5</v>
@@ -1486,10 +1280,10 @@
         <v>0.3</v>
       </c>
       <c r="G33">
-        <v>-264.64158800000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-472.092968</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1497,7 +1291,7 @@
         <v>38</v>
       </c>
       <c r="C34">
-        <v>449</v>
+        <v>192</v>
       </c>
       <c r="D34">
         <v>5</v>
@@ -1509,22 +1303,10 @@
         <v>0.3</v>
       </c>
       <c r="G34">
-        <v>-252.36460099999999</v>
-      </c>
-      <c r="H34">
-        <f>C34</f>
-        <v>449</v>
-      </c>
-      <c r="I34">
-        <f>AVERAGE(G34:G39)</f>
-        <v>-253.47181516666669</v>
-      </c>
-      <c r="J34">
-        <f>_xlfn.STDEV.P(G34:G39)</f>
-        <v>1.2747305032537219</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-247.310736</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1532,7 +1314,7 @@
         <v>39</v>
       </c>
       <c r="C35">
-        <v>449</v>
+        <v>364</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -1544,10 +1326,10 @@
         <v>0.3</v>
       </c>
       <c r="G35">
-        <v>-251.89984899999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-280.558068</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1555,7 +1337,7 @@
         <v>40</v>
       </c>
       <c r="C36">
-        <v>449</v>
+        <v>192</v>
       </c>
       <c r="D36">
         <v>5</v>
@@ -1567,10 +1349,10 @@
         <v>0.3</v>
       </c>
       <c r="G36">
-        <v>-253.55488</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-245.233356</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1578,7 +1360,7 @@
         <v>41</v>
       </c>
       <c r="C37">
-        <v>449</v>
+        <v>71</v>
       </c>
       <c r="D37">
         <v>5</v>
@@ -1590,10 +1372,10 @@
         <v>0.3</v>
       </c>
       <c r="G37">
-        <v>-252.855909</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-473.105508</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1601,7 +1383,7 @@
         <v>42</v>
       </c>
       <c r="C38">
-        <v>449</v>
+        <v>371</v>
       </c>
       <c r="D38">
         <v>5</v>
@@ -1613,10 +1395,10 @@
         <v>0.3</v>
       </c>
       <c r="G38">
-        <v>-254.57391899999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-265.320402</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1624,7 +1406,7 @@
         <v>43</v>
       </c>
       <c r="C39">
-        <v>449</v>
+        <v>364</v>
       </c>
       <c r="D39">
         <v>5</v>
@@ -1636,10 +1418,10 @@
         <v>0.3</v>
       </c>
       <c r="G39">
-        <v>-255.58173300000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-284.627274</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1647,7 +1429,7 @@
         <v>44</v>
       </c>
       <c r="C40">
-        <v>700</v>
+        <v>364</v>
       </c>
       <c r="D40">
         <v>5</v>
@@ -1659,22 +1441,10 @@
         <v>0.3</v>
       </c>
       <c r="G40">
-        <v>-261.79965399999998</v>
-      </c>
-      <c r="H40">
-        <f>C40</f>
-        <v>700</v>
-      </c>
-      <c r="I40">
-        <f>AVERAGE(G40:G45)</f>
-        <v>-263.69524166666667</v>
-      </c>
-      <c r="J40">
-        <f>_xlfn.STDEV.P(G40:G45)</f>
-        <v>3.3137798215478336</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-281.372597</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1682,7 +1452,7 @@
         <v>45</v>
       </c>
       <c r="C41">
-        <v>700</v>
+        <v>536</v>
       </c>
       <c r="D41">
         <v>5</v>
@@ -1694,10 +1464,10 @@
         <v>0.3</v>
       </c>
       <c r="G41">
-        <v>-262.63329399999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-276.568297</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1705,7 +1475,7 @@
         <v>46</v>
       </c>
       <c r="C42">
-        <v>700</v>
+        <v>71</v>
       </c>
       <c r="D42">
         <v>5</v>
@@ -1717,10 +1487,10 @@
         <v>0.3</v>
       </c>
       <c r="G42">
-        <v>-257.79432700000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-474.035134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1728,7 +1498,7 @@
         <v>47</v>
       </c>
       <c r="C43">
-        <v>700</v>
+        <v>100</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -1740,10 +1510,10 @@
         <v>0.3</v>
       </c>
       <c r="G43">
-        <v>-266.336142</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-580.643008</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1751,7 +1521,7 @@
         <v>48</v>
       </c>
       <c r="C44">
-        <v>700</v>
+        <v>371</v>
       </c>
       <c r="D44">
         <v>5</v>
@@ -1763,10 +1533,10 @@
         <v>0.3</v>
       </c>
       <c r="G44">
-        <v>-266.65957900000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-264.641588</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1774,7 +1544,7 @@
         <v>49</v>
       </c>
       <c r="C45">
-        <v>700</v>
+        <v>137</v>
       </c>
       <c r="D45">
         <v>5</v>
@@ -1786,11 +1556,10 @@
         <v>0.3</v>
       </c>
       <c r="G45">
-        <v>-266.94845400000003</v>
+        <v>-456.997681</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>